<commit_message>
Write tests for unmapped profiles
</commit_message>
<xml_diff>
--- a/Ubuntu VM Test Results.xlsx
+++ b/Ubuntu VM Test Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RGOVIND\Documents\canonical-ubuntu-22.04-lts-stig-baseline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEA0B077-FE3C-43DD-80AD-65475733D15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5645AB37-1807-42C7-8A0B-B0B52F0CAD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{541800BB-D781-9C45-B99B-06442BC9A2C7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="830">
   <si>
     <t>Rhel 9 Controls</t>
   </si>
@@ -2463,39 +2463,12 @@
     <t>N/A - tests don't exist</t>
   </si>
   <si>
-    <t>2 successful, 1  failure</t>
-  </si>
-  <si>
-    <t>1 successful, 2 failure</t>
-  </si>
-  <si>
-    <t>2 succesful, 1 failure</t>
-  </si>
-  <si>
-    <t>1 successful, 1 failure</t>
-  </si>
-  <si>
-    <t>2 successful, 3 failures</t>
-  </si>
-  <si>
     <t>1/1 test failure</t>
   </si>
   <si>
-    <t>1/1 tests working</t>
-  </si>
-  <si>
-    <t>2/2 successful tests</t>
-  </si>
-  <si>
     <t>3/3 test failures</t>
   </si>
   <si>
-    <t>1/1 successful test</t>
-  </si>
-  <si>
-    <t>1 successful, 2 failures</t>
-  </si>
-  <si>
     <t>1/1 skipped test</t>
   </si>
   <si>
@@ -2511,27 +2484,12 @@
     <t>1/1 skipped test - manual check required</t>
   </si>
   <si>
-    <t>1 successful, 3 failures</t>
-  </si>
-  <si>
     <t>1/1 test failure (test works)</t>
   </si>
   <si>
-    <t>3 test failures (tests work)</t>
-  </si>
-  <si>
     <t>1/1 test failure (sshd client alive count max has no value)</t>
   </si>
   <si>
-    <t>1/1 test failure (works)</t>
-  </si>
-  <si>
-    <t>1/1 tests failed (test works)</t>
-  </si>
-  <si>
-    <t>2/2 test failures (test works)</t>
-  </si>
-  <si>
     <t>1/1 test failure (rewrite)</t>
   </si>
   <si>
@@ -2560,6 +2518,15 @@
   </si>
   <si>
     <t>rewritten</t>
+  </si>
+  <si>
+    <t>auditd.conf not found</t>
+  </si>
+  <si>
+    <t>works - manual check needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">works </t>
   </si>
 </sst>
 </file>
@@ -2587,7 +2554,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2612,6 +2579,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2625,7 +2598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2633,6 +2606,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2984,8 +2959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9E95DE-A35F-D24C-B26F-063E6D2CD261}">
   <dimension ref="A1:D184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3020,7 +2995,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>833</v>
+        <v>819</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3031,7 +3006,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>834</v>
+        <v>820</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3064,7 +3039,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>808</v>
+        <v>825</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3075,7 +3050,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>809</v>
+        <v>825</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3086,7 +3061,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>810</v>
+        <v>825</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3110,6 +3085,9 @@
       <c r="C10" t="s">
         <v>696</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -3121,6 +3099,9 @@
       <c r="C11" t="s">
         <v>697</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -3132,6 +3113,9 @@
       <c r="C12" t="s">
         <v>698</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3154,6 +3138,9 @@
       <c r="C14" t="s">
         <v>699</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -3165,6 +3152,9 @@
       <c r="C15" t="s">
         <v>700</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -3174,7 +3164,7 @@
         <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -3185,7 +3175,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -3196,7 +3186,7 @@
         <v>104</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -3229,7 +3219,7 @@
         <v>109</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -3240,7 +3230,7 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3254,7 +3244,7 @@
         <v>705</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>811</v>
+        <v>825</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -3267,6 +3257,9 @@
       <c r="C24" t="s">
         <v>706</v>
       </c>
+      <c r="D24" s="4" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -3275,6 +3268,9 @@
       <c r="B25" t="s">
         <v>470</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -3284,7 +3280,7 @@
         <v>112</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -3295,7 +3291,7 @@
         <v>143</v>
       </c>
       <c r="D27" t="s">
-        <v>836</v>
+        <v>822</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -3323,7 +3319,7 @@
         <v>712</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -3334,7 +3330,7 @@
         <v>144</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -3345,7 +3341,7 @@
         <v>147</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -3356,7 +3352,7 @@
         <v>148</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3367,7 +3363,7 @@
         <v>145</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3378,7 +3374,7 @@
         <v>146</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -3466,7 +3462,7 @@
         <v>139</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>815</v>
+        <v>825</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -3480,7 +3476,7 @@
         <v>719</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>811</v>
+        <v>825</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3493,6 +3489,9 @@
       <c r="C44" t="s">
         <v>721</v>
       </c>
+      <c r="D44" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -3504,6 +3503,9 @@
       <c r="C45" t="s">
         <v>720</v>
       </c>
+      <c r="D45" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -3524,7 +3526,7 @@
         <v>723</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -3538,7 +3540,7 @@
         <v>724</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -3551,6 +3553,9 @@
       <c r="C49" t="s">
         <v>725</v>
       </c>
+      <c r="D49" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -3577,7 +3582,7 @@
         <v>774</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>837</v>
+        <v>823</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -3588,7 +3593,7 @@
         <v>165</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -3599,7 +3604,7 @@
         <v>170</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>838</v>
+        <v>824</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -3612,6 +3617,9 @@
       <c r="C54" t="s">
         <v>775</v>
       </c>
+      <c r="D54" s="2" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
@@ -3623,6 +3631,9 @@
       <c r="C55" t="s">
         <v>776</v>
       </c>
+      <c r="D55" s="2" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -3632,7 +3643,7 @@
         <v>182</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>808</v>
+        <v>825</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -3643,7 +3654,7 @@
         <v>203</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -3654,7 +3665,7 @@
         <v>204</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -3668,7 +3679,7 @@
         <v>777</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>811</v>
+        <v>825</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -3679,7 +3690,7 @@
         <v>218</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -3690,7 +3701,7 @@
         <v>220</v>
       </c>
       <c r="D61" t="s">
-        <v>827</v>
+        <v>816</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -3701,7 +3712,7 @@
         <v>221</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -3712,7 +3723,7 @@
         <v>232</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -3723,7 +3734,7 @@
         <v>236</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -3745,7 +3756,7 @@
         <v>216</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>839</v>
+        <v>825</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -3778,7 +3789,7 @@
         <v>237</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -3789,7 +3800,7 @@
         <v>237</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>839</v>
+        <v>825</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -3803,7 +3814,7 @@
         <v>781</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>840</v>
+        <v>826</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -3814,7 +3825,7 @@
         <v>248</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>839</v>
+        <v>825</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -3828,7 +3839,7 @@
         <v>782</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>840</v>
+        <v>826</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -3841,6 +3852,9 @@
       <c r="C74" t="s">
         <v>783</v>
       </c>
+      <c r="D74" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -3850,7 +3864,7 @@
         <v>265</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -3872,7 +3886,7 @@
         <v>270</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -3894,7 +3908,7 @@
         <v>329</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3905,7 +3919,7 @@
         <v>266</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -3916,7 +3930,7 @@
         <v>274</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>812</v>
+        <v>825</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -3927,7 +3941,7 @@
         <v>272</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -3949,7 +3963,7 @@
         <v>296</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>840</v>
+        <v>826</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -3960,7 +3974,7 @@
         <v>301</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>840</v>
+        <v>826</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -3971,7 +3985,7 @@
         <v>294</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>811</v>
+        <v>825</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -3993,7 +4007,7 @@
         <v>291</v>
       </c>
       <c r="D88" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -4004,7 +4018,7 @@
         <v>299</v>
       </c>
       <c r="D89" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -4037,7 +4051,7 @@
         <v>311</v>
       </c>
       <c r="D92" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -4059,7 +4073,7 @@
         <v>336</v>
       </c>
       <c r="D94" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -4070,7 +4084,7 @@
         <v>327</v>
       </c>
       <c r="D95" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -4081,7 +4095,7 @@
         <v>328</v>
       </c>
       <c r="D96" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -4092,7 +4106,7 @@
         <v>334</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>818</v>
+        <v>825</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -4103,7 +4117,7 @@
         <v>335</v>
       </c>
       <c r="D98" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -4114,7 +4128,7 @@
         <v>332</v>
       </c>
       <c r="D99" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -4125,7 +4139,7 @@
         <v>337</v>
       </c>
       <c r="D100" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -4161,7 +4175,7 @@
         <v>476</v>
       </c>
       <c r="D103" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -4172,7 +4186,7 @@
         <v>319</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -4183,7 +4197,7 @@
         <v>345</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -4194,7 +4208,7 @@
         <v>456</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -4255,7 +4269,7 @@
         <v>356</v>
       </c>
       <c r="D111" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -4280,7 +4294,7 @@
         <v>357</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -4305,7 +4319,7 @@
         <v>797</v>
       </c>
       <c r="D115" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -4316,7 +4330,7 @@
         <v>359</v>
       </c>
       <c r="D116" t="s">
-        <v>831</v>
+        <v>817</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -4335,7 +4349,7 @@
         <v>360</v>
       </c>
       <c r="D118" t="s">
-        <v>832</v>
+        <v>818</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -4354,7 +4368,7 @@
         <v>362</v>
       </c>
       <c r="D120" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -4373,7 +4387,7 @@
         <v>365</v>
       </c>
       <c r="D122" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -4384,7 +4398,7 @@
         <v>369</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -4409,7 +4423,7 @@
         <v>799</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -4422,8 +4436,8 @@
       <c r="C126" t="s">
         <v>800</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>825</v>
+      <c r="D126" s="6" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -4436,6 +4450,9 @@
       <c r="C127" t="s">
         <v>773</v>
       </c>
+      <c r="D127" s="5" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
@@ -4447,8 +4464,11 @@
       <c r="C128" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>640</v>
       </c>
@@ -4458,8 +4478,11 @@
       <c r="C129" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129" s="3" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>641</v>
       </c>
@@ -4469,8 +4492,11 @@
       <c r="C130" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130" s="3" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>642</v>
       </c>
@@ -4480,8 +4506,11 @@
       <c r="C131" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131" s="3" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>643</v>
       </c>
@@ -4491,8 +4520,11 @@
       <c r="C132" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>644</v>
       </c>
@@ -4502,8 +4534,11 @@
       <c r="C133" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>645</v>
       </c>
@@ -4514,7 +4549,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>646</v>
       </c>
@@ -4524,8 +4559,11 @@
       <c r="C135" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135" s="3" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>647</v>
       </c>
@@ -4536,7 +4574,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>648</v>
       </c>
@@ -4547,7 +4585,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>649</v>
       </c>
@@ -4558,7 +4596,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>650</v>
       </c>
@@ -4569,7 +4607,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>651</v>
       </c>
@@ -4580,7 +4618,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>652</v>
       </c>
@@ -4591,7 +4629,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>653</v>
       </c>
@@ -4602,7 +4640,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>654</v>
       </c>
@@ -4613,7 +4651,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>655</v>
       </c>

</xml_diff>

<commit_message>
Manually write controls and add inputs.yml
</commit_message>
<xml_diff>
--- a/Ubuntu VM Test Results.xlsx
+++ b/Ubuntu VM Test Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RGOVIND\Documents\canonical-ubuntu-22.04-lts-stig-baseline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5645AB37-1807-42C7-8A0B-B0B52F0CAD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74F4C81-1468-4AF7-8C71-B6ECC40435D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{541800BB-D781-9C45-B99B-06442BC9A2C7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="831">
   <si>
     <t>Rhel 9 Controls</t>
   </si>
@@ -2527,6 +2527,9 @@
   </si>
   <si>
     <t xml:space="preserve">works </t>
+  </si>
+  <si>
+    <t>not sure (SV-255912 on 20.04)</t>
   </si>
 </sst>
 </file>
@@ -2959,8 +2962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9E95DE-A35F-D24C-B26F-063E6D2CD261}">
   <dimension ref="A1:D184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3747,6 +3750,9 @@
       <c r="C65" t="s">
         <v>778</v>
       </c>
+      <c r="D65" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -3769,6 +3775,9 @@
       <c r="C67" t="s">
         <v>780</v>
       </c>
+      <c r="D67" s="4" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
@@ -3780,6 +3789,9 @@
       <c r="C68" t="s">
         <v>779</v>
       </c>
+      <c r="D68" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -3877,6 +3889,9 @@
       <c r="C76" t="s">
         <v>784</v>
       </c>
+      <c r="D76" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -3899,6 +3914,9 @@
       <c r="C78" t="s">
         <v>785</v>
       </c>
+      <c r="D78" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -3998,6 +4016,9 @@
       <c r="C87" t="s">
         <v>786</v>
       </c>
+      <c r="D87" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
@@ -4031,6 +4052,9 @@
       <c r="C90" t="s">
         <v>787</v>
       </c>
+      <c r="D90" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
@@ -4042,6 +4066,9 @@
       <c r="C91" t="s">
         <v>788</v>
       </c>
+      <c r="D91" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
@@ -4064,6 +4091,9 @@
       <c r="C93" t="s">
         <v>789</v>
       </c>
+      <c r="D93" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
@@ -4152,6 +4182,9 @@
       <c r="C101" t="s">
         <v>790</v>
       </c>
+      <c r="D101" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
@@ -4163,6 +4196,9 @@
       <c r="C102" t="s">
         <v>791</v>
       </c>
+      <c r="D102" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
@@ -4249,6 +4285,9 @@
       <c r="C109" t="s">
         <v>794</v>
       </c>
+      <c r="D109" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
@@ -4259,6 +4298,9 @@
       </c>
       <c r="C110" t="s">
         <v>795</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>